<commit_message>
added cardkingdom and ebay buy it now to avoid errors when tcgplayer mid/market are not availible. Cleaned code a bit and am now testing day to day automation and  average/daily change columns (I need different data values to test and don't feel like mocking data lol)
</commit_message>
<xml_diff>
--- a/excels/my_list_report.xlsx
+++ b/excels/my_list_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Card name</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Daily Change</t>
   </si>
   <si>
-    <t>Price 2021-05-11</t>
+    <t>Price 2021-05-12</t>
   </si>
   <si>
     <t>Intuition, Tempest (TE) Price History</t>
@@ -82,58 +82,49 @@
     <t>Boseiju Who Shelters All, From the Vault Realms:Foil (V12) Price</t>
   </si>
   <si>
-    <t>194.70</t>
-  </si>
-  <si>
-    <t>0.31</t>
-  </si>
-  <si>
-    <t>16.21</t>
-  </si>
-  <si>
-    <t>4.19</t>
-  </si>
-  <si>
-    <t>37.50</t>
-  </si>
-  <si>
-    <t>21.09</t>
-  </si>
-  <si>
-    <t>19.75</t>
-  </si>
-  <si>
-    <t>6.39</t>
-  </si>
-  <si>
-    <t>5.27</t>
-  </si>
-  <si>
-    <t>14.64</t>
-  </si>
-  <si>
-    <t>5.76</t>
-  </si>
-  <si>
-    <t>5.43</t>
-  </si>
-  <si>
-    <t>10.29</t>
-  </si>
-  <si>
-    <t>3.24</t>
-  </si>
-  <si>
-    <t>11.16</t>
-  </si>
-  <si>
-    <t>11.88</t>
-  </si>
-  <si>
-    <t>58.50</t>
-  </si>
-  <si>
-    <t>28.26</t>
+    <t>249.99</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>20.99</t>
+  </si>
+  <si>
+    <t>5.99</t>
+  </si>
+  <si>
+    <t>39.99</t>
+  </si>
+  <si>
+    <t>26.99</t>
+  </si>
+  <si>
+    <t>22.99</t>
+  </si>
+  <si>
+    <t>7.99</t>
+  </si>
+  <si>
+    <t>12.99</t>
+  </si>
+  <si>
+    <t>3.49</t>
+  </si>
+  <si>
+    <t>4.49</t>
+  </si>
+  <si>
+    <t>8.49</t>
+  </si>
+  <si>
+    <t>10.99</t>
+  </si>
+  <si>
+    <t>89.99</t>
+  </si>
+  <si>
+    <t>27.99</t>
   </si>
 </sst>
 </file>
@@ -634,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -648,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -662,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -676,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -690,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -704,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -718,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -732,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -746,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -760,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pop up messages for single cards that match an operator price in my_list.txt. added settings.txt functionality which lets you run operators against the price, daily price, daily percent price, weekly price, and weekly percent price. See Readme for more details.
</commit_message>
<xml_diff>
--- a/excels/my_list_report.xlsx
+++ b/excels/my_list_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Card name</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Highest Price</t>
   </si>
   <si>
-    <t>Price 2021-05-17</t>
+    <t>Price 2021-05-23</t>
   </si>
   <si>
     <t>Intuition, Tempest (TE) Price History</t>
@@ -50,54 +50,6 @@
   </si>
   <si>
     <t>Demonic Consultation, Ice Age (ICE) Price History</t>
-  </si>
-  <si>
-    <t>Gamble, Judge Promos:Foil (PRM-JUD) Price History</t>
-  </si>
-  <si>
-    <t>Rain of Filth, Urzas Saga (UZ) Price History</t>
-  </si>
-  <si>
-    <t>Red Elemental Blast, Revised Edition (3ED) Price History</t>
-  </si>
-  <si>
-    <t>Brain Freeze, The List (PLIST) Price History</t>
-  </si>
-  <si>
-    <t>Cabal Ritual, Torment (TOR) Price History</t>
-  </si>
-  <si>
-    <t>Snap, Mystery Booster (MB1) Price History</t>
-  </si>
-  <si>
-    <t>Winds of Rebuke, Amonkhet (AKH) Price History</t>
-  </si>
-  <si>
-    <t>Praetors Grasp, New Phyrexia (NPH) Price History</t>
-  </si>
-  <si>
-    <t>Wheel of Misfortune, Commander Legends (CMR) Price History</t>
-  </si>
-  <si>
-    <t>Ad Nauseam, Double Masters (2XM) Price History</t>
-  </si>
-  <si>
-    <t>Peer into the Abyss, Core Set 2021 (M21) Price History</t>
-  </si>
-  <si>
-    <t>Talisman of Creativity, Commander 2021 (C21) Price History</t>
-  </si>
-  <si>
-    <t>Talisman of Dominance, Mirrodin (MRD) Price History</t>
-  </si>
-  <si>
-    <t>Underworld Breach, Theros Beyond Death (THB) Price History</t>
-  </si>
-  <si>
-    <t>Boseiju Who Shelters All, From the Vault Realms:Foil (V12) Price</t>
-  </si>
-  <si>
-    <t>Spire of Industry, Aether Revolt (AER) Price History</t>
   </si>
 </sst>
 </file>
@@ -455,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -504,7 +456,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>239.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -527,7 +479,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -596,12 +548,12 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>26.99</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -619,357 +571,12 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>32.94</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>2.29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>6.99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>4.99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>4.49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>1.49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>1.49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>24.99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>1.99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="G23">
-        <v>438.2400000000001</v>
+        <v>291.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new gmail functionality
</commit_message>
<xml_diff>
--- a/excels/my_list_report.xlsx
+++ b/excels/my_list_report.xlsx
@@ -34,7 +34,7 @@
     <t>Highest Price</t>
   </si>
   <si>
-    <t>Price 2021-05-23</t>
+    <t>Price 2021-05-30</t>
   </si>
   <si>
     <t>Intuition, Tempest (TE) Price History</t>
@@ -502,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>20.99</v>
+        <v>19.99</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -525,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>17.99</v>
+        <v>19.99</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -576,7 +576,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="G8">
-        <v>291.3</v>
+        <v>292.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>